<commit_message>
example with comparison of calculations
example of detailed calculations of s2 without using VAR.S function

(to be deleted after checked by user)

#23
</commit_message>
<xml_diff>
--- a/estimSppComp.xlsx
+++ b/estimSppComp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WORK\Design&amp;Analysis\SampleSizeUnsorted\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7092DCB3-0AB6-493E-9A19-BFE1546BA249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C40FB2C-D211-4DAA-A810-FC0BD25DB578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27330" yWindow="1470" windowWidth="21600" windowHeight="12405" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="7" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
   <si>
     <t>Sample No</t>
   </si>
@@ -134,6 +134,27 @@
   <si>
     <t>main results are displayed in bold (species estimates in proportion and weight; sample size estimated to attain the error margin)</t>
   </si>
+  <si>
+    <t>squared errors</t>
+  </si>
+  <si>
+    <t>comparison R33 vs R52</t>
+  </si>
+  <si>
+    <t>sum of squared errors / 13</t>
+  </si>
+  <si>
+    <t>-&gt; R3^2</t>
+  </si>
+  <si>
+    <t>-&gt; =SUM(R36:R49)/13</t>
+  </si>
+  <si>
+    <t>-&gt; R16^2</t>
+  </si>
+  <si>
+    <t>-&gt; =S51=R33</t>
+  </si>
 </sst>
 </file>
 
@@ -207,7 +228,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -250,6 +271,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="21">
     <border>
@@ -520,7 +547,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -650,6 +677,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -728,6 +757,64 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>311727</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>311727</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>155864</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D08A41C-3B77-4175-EAED-11DB49302F07}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13092545" y="6641523"/>
+          <a:ext cx="0" cy="2086841"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1045,12 +1132,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB49"/>
+  <dimension ref="A1:AB54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I36" sqref="I36"/>
-      <selection pane="bottomLeft" activeCell="C49" sqref="C49"/>
+      <selection pane="bottomLeft" activeCell="T54" sqref="T54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1058,11 +1145,13 @@
     <col min="1" max="1" width="9.73046875" customWidth="1"/>
     <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.1328125" customWidth="1"/>
-    <col min="4" max="7" width="20.1328125" customWidth="1"/>
-    <col min="8" max="13" width="20.1328125" style="5" customWidth="1"/>
+    <col min="4" max="6" width="20.1328125" customWidth="1"/>
+    <col min="7" max="7" width="20.1328125" hidden="1" customWidth="1"/>
+    <col min="8" max="13" width="20.1328125" style="5" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="10.59765625" style="5" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="22.73046875" customWidth="1"/>
     <col min="17" max="17" width="23.3984375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.46484375" customWidth="1"/>
     <col min="27" max="27" width="21" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="21" customWidth="1"/>
   </cols>
@@ -3199,7 +3288,11 @@
       <c r="L34" s="32"/>
       <c r="M34" s="32"/>
     </row>
-    <row r="35" spans="1:27" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="35" spans="1:27" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="R35" t="s">
+        <v>32</v>
+      </c>
+    </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A36" s="23"/>
       <c r="B36" s="24" t="s">
@@ -3238,6 +3331,13 @@
       <c r="M36" s="26" t="s">
         <v>13</v>
       </c>
+      <c r="R36">
+        <f>R3^2</f>
+        <v>0.22066532203046194</v>
+      </c>
+      <c r="S36" s="66" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A37" s="57" t="s">
@@ -3289,6 +3389,10 @@
       <c r="M37" s="48">
         <f t="shared" si="24"/>
         <v>0</v>
+      </c>
+      <c r="R37">
+        <f>R4^2</f>
+        <v>3.4048201293000568E-2</v>
       </c>
     </row>
     <row r="38" spans="1:27" x14ac:dyDescent="0.45">
@@ -3337,6 +3441,10 @@
         <f t="shared" si="25"/>
         <v/>
       </c>
+      <c r="R38">
+        <f>R5^2</f>
+        <v>0.21580901242330705</v>
+      </c>
     </row>
     <row r="39" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A39" s="57"/>
@@ -3384,6 +3492,10 @@
         <f t="shared" si="26"/>
         <v/>
       </c>
+      <c r="R39">
+        <f>R6^2</f>
+        <v>0.17562119300387585</v>
+      </c>
     </row>
     <row r="40" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A40" s="57"/>
@@ -3430,6 +3542,10 @@
       <c r="M40" s="56" t="str">
         <f t="shared" si="27"/>
         <v/>
+      </c>
+      <c r="R40">
+        <f>R7^2</f>
+        <v>0.26814773724367225</v>
       </c>
     </row>
     <row r="41" spans="1:27" x14ac:dyDescent="0.45">
@@ -3445,6 +3561,10 @@
       <c r="K41" s="10"/>
       <c r="L41" s="10"/>
       <c r="M41" s="50"/>
+      <c r="R41">
+        <f>R8^2</f>
+        <v>2.9578982754177234</v>
+      </c>
     </row>
     <row r="42" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="58" t="s">
@@ -3496,6 +3616,10 @@
       <c r="M42" s="52">
         <f t="shared" si="28"/>
         <v>0</v>
+      </c>
+      <c r="R42">
+        <f>R9^2</f>
+        <v>0.2286720696242473</v>
       </c>
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.45">
@@ -3544,6 +3668,10 @@
         <f t="shared" si="29"/>
         <v/>
       </c>
+      <c r="R43">
+        <f>R10^2</f>
+        <v>3.2859874489789428E-2</v>
+      </c>
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A44" s="58"/>
@@ -3591,6 +3719,10 @@
         <f t="shared" si="30"/>
         <v/>
       </c>
+      <c r="R44">
+        <f>R11^2</f>
+        <v>0.21280125808125397</v>
+      </c>
     </row>
     <row r="45" spans="1:27" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A45" s="59"/>
@@ -3638,8 +3770,17 @@
         <f t="shared" si="31"/>
         <v/>
       </c>
-    </row>
-    <row r="46" spans="1:27" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+      <c r="R45">
+        <f>R12^2</f>
+        <v>0.13619280517200227</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="R46">
+        <f>R13^2</f>
+        <v>0.2286720696242473</v>
+      </c>
+    </row>
     <row r="47" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A47" s="13"/>
       <c r="B47" s="19" t="s">
@@ -3676,6 +3817,10 @@
       <c r="M47" s="15" t="s">
         <v>13</v>
       </c>
+      <c r="R47">
+        <f>R14^2</f>
+        <v>7.8724330315875664</v>
+      </c>
     </row>
     <row r="48" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A48" s="16"/>
@@ -3725,8 +3870,12 @@
         <f t="shared" si="32"/>
         <v/>
       </c>
-    </row>
-    <row r="49" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="R48">
+        <f>R15^2</f>
+        <v>0.18110902548762106</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A49" s="17"/>
       <c r="B49" s="21" t="s">
         <v>24</v>
@@ -3773,6 +3922,37 @@
       <c r="M49" s="22" t="str">
         <f t="shared" si="33"/>
         <v/>
+      </c>
+      <c r="R49">
+        <f>R16^2</f>
+        <v>5.8264966270870121E-3</v>
+      </c>
+      <c r="S49" s="66" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="R51" t="s">
+        <v>34</v>
+      </c>
+      <c r="S51">
+        <f>SUM(R36:R49)/13</f>
+        <v>0.98236587477737358</v>
+      </c>
+      <c r="T51" s="66" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="R54" t="s">
+        <v>33</v>
+      </c>
+      <c r="S54" s="65" t="b">
+        <f>S51=R33</f>
+        <v>1</v>
+      </c>
+      <c r="T54" s="66" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -3785,5 +3965,6 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>